<commit_message>
japan other food data
</commit_message>
<xml_diff>
--- a/data-raw/nutr_key.xlsx
+++ b/data-raw/nutr_key.xlsx
@@ -245,13 +245,13 @@
     <t>fatty acid poly unsaturated</t>
   </si>
   <si>
-    <t>Polyunsaturated fatty acids: Linoleic acid (omega 6)</t>
+    <t>Linoleic acid</t>
   </si>
   <si>
     <t>fatty acid 18 2 n 6</t>
   </si>
   <si>
-    <t>Polyunsaturated fatty acids: α -Linolenic acid (omega 3)</t>
+    <t>α -Linolenic acid</t>
   </si>
   <si>
     <t>fatty acid 18 3 n 3</t>
@@ -275,7 +275,7 @@
     <t>iron</t>
   </si>
   <si>
-    <t>Magnesium~</t>
+    <t>Magnesium</t>
   </si>
   <si>
     <t>magnesium</t>

</xml_diff>